<commit_message>
Agrega hasta 3.13 y limpia base hasta 3.20
</commit_message>
<xml_diff>
--- a/Codigo/Bases/datos_administrativos/Indicadores_de_Género/EDUCACIÓN/EducaciónSinFormato.xlsx
+++ b/Codigo/Bases/datos_administrativos/Indicadores_de_Género/EDUCACIÓN/EducaciónSinFormato.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pgalvez\OneDrive - ine.gob.gt\Documentos\GitHub\CompendioGenero2023\Codigo\Bases\datos_administrativos\Indicadores_de_Género\EDUCACIÓN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1D65A6-EBFF-4F88-A96E-6BD58B7F9B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000C8E67-AF65-4071-9456-A5055D4F3F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="8" activeTab="17" xr2:uid="{47FD8A6C-84B7-4DDA-B99C-2C5D2BD14377}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="10" xr2:uid="{47FD8A6C-84B7-4DDA-B99C-2C5D2BD14377}"/>
   </bookViews>
   <sheets>
     <sheet name="3.4" sheetId="20" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="41">
   <si>
     <t>Sexo</t>
   </si>
@@ -162,6 +162,21 @@
   <si>
     <t>Suchitepéquez</t>
   </si>
+  <si>
+    <t>Tasa</t>
+  </si>
+  <si>
+    <t>Porcentaje</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Nivel</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
 </sst>
 </file>
 
@@ -199,10 +214,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,7 +611,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,22 +621,22 @@
         <v>23</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
       <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -628,22 +644,22 @@
         <v>5</v>
       </c>
       <c r="B2">
+        <v>8.5503298346820493</v>
+      </c>
+      <c r="C2">
         <v>13.386533007979951</v>
       </c>
-      <c r="C2">
-        <v>8.5503298346820493</v>
-      </c>
       <c r="D2">
+        <v>7.9299849747653113</v>
+      </c>
+      <c r="E2">
         <v>12.873754152823921</v>
       </c>
-      <c r="E2">
-        <v>7.9299849747653113</v>
-      </c>
       <c r="F2">
+        <v>5.9091027885947254</v>
+      </c>
+      <c r="G2">
         <v>9.4187312117756807</v>
-      </c>
-      <c r="G2">
-        <v>5.9091027885947254</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -651,22 +667,22 @@
         <v>6</v>
       </c>
       <c r="B3">
+        <v>9.8314606741573041</v>
+      </c>
+      <c r="C3">
         <v>13.957816377171216</v>
       </c>
-      <c r="C3">
-        <v>9.8314606741573041</v>
-      </c>
       <c r="D3">
+        <v>9.1846013943619287</v>
+      </c>
+      <c r="E3">
         <v>12.580744386342662</v>
       </c>
-      <c r="E3">
-        <v>9.1846013943619287</v>
-      </c>
       <c r="F3">
+        <v>4.6518792359827472</v>
+      </c>
+      <c r="G3">
         <v>6.963366636391159</v>
-      </c>
-      <c r="G3">
-        <v>4.6518792359827472</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -674,22 +690,22 @@
         <v>32</v>
       </c>
       <c r="B4">
+        <v>7.7618908666472128</v>
+      </c>
+      <c r="C4">
         <v>12.128995433789955</v>
       </c>
-      <c r="C4">
-        <v>7.7618908666472128</v>
-      </c>
       <c r="D4">
+        <v>6.3956714761376254</v>
+      </c>
+      <c r="E4">
         <v>10.910593745695</v>
       </c>
-      <c r="E4">
-        <v>6.3956714761376254</v>
-      </c>
       <c r="F4">
+        <v>3.4182120121782456</v>
+      </c>
+      <c r="G4">
         <v>6.8091732729331822</v>
-      </c>
-      <c r="G4">
-        <v>3.4182120121782456</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -697,22 +713,22 @@
         <v>7</v>
       </c>
       <c r="B5">
+        <v>0.77594663527565233</v>
+      </c>
+      <c r="C5">
         <v>10.615188024826578</v>
       </c>
-      <c r="C5">
-        <v>0.77594663527565233</v>
-      </c>
       <c r="D5">
+        <v>5.8219509832413054</v>
+      </c>
+      <c r="E5">
         <v>9.3237983162849645</v>
       </c>
-      <c r="E5">
-        <v>5.8219509832413054</v>
-      </c>
       <c r="F5">
+        <v>5.6536420646406178</v>
+      </c>
+      <c r="G5">
         <v>8.7363775556155989</v>
-      </c>
-      <c r="G5">
-        <v>5.6536420646406178</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -720,22 +736,22 @@
         <v>8</v>
       </c>
       <c r="B6">
+        <v>9.2958640946257045</v>
+      </c>
+      <c r="C6">
         <v>12.238087847276113</v>
       </c>
-      <c r="C6">
-        <v>9.2958640946257045</v>
-      </c>
       <c r="D6">
+        <v>8.2727008149010484</v>
+      </c>
+      <c r="E6">
         <v>11.073205401563611</v>
       </c>
-      <c r="E6">
-        <v>8.2727008149010484</v>
-      </c>
       <c r="F6">
+        <v>3.3365250055240478</v>
+      </c>
+      <c r="G6">
         <v>4.6245226983453538</v>
-      </c>
-      <c r="G6">
-        <v>3.3365250055240478</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -743,22 +759,22 @@
         <v>9</v>
       </c>
       <c r="B7">
+        <v>6.2534741523068371</v>
+      </c>
+      <c r="C7">
         <v>8.6109090909090913</v>
       </c>
-      <c r="C7">
-        <v>6.2534741523068371</v>
-      </c>
       <c r="D7">
+        <v>7.4940836181961608</v>
+      </c>
+      <c r="E7">
         <v>10.9375</v>
       </c>
-      <c r="E7">
-        <v>7.4940836181961608</v>
-      </c>
       <c r="F7">
+        <v>4.9993316401550594</v>
+      </c>
+      <c r="G7">
         <v>5.5623889572229057</v>
-      </c>
-      <c r="G7">
-        <v>4.9993316401550594</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -766,22 +782,22 @@
         <v>33</v>
       </c>
       <c r="B8">
+        <v>5.7507082152974505</v>
+      </c>
+      <c r="C8">
         <v>9.0216186252771617</v>
       </c>
-      <c r="C8">
-        <v>5.7507082152974505</v>
-      </c>
       <c r="D8">
+        <v>4.1123085649461144</v>
+      </c>
+      <c r="E8">
         <v>7.7273983964611563</v>
       </c>
-      <c r="E8">
-        <v>4.1123085649461144</v>
-      </c>
       <c r="F8">
+        <v>4.7309702019488773</v>
+      </c>
+      <c r="G8">
         <v>6.5800502933780383</v>
-      </c>
-      <c r="G8">
-        <v>4.7309702019488773</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -789,22 +805,22 @@
         <v>34</v>
       </c>
       <c r="B9">
+        <v>7.0540935672514626</v>
+      </c>
+      <c r="C9">
         <v>9.5462184873949578</v>
       </c>
-      <c r="C9">
-        <v>7.0540935672514626</v>
-      </c>
       <c r="D9">
+        <v>5.8387395736793328</v>
+      </c>
+      <c r="E9">
         <v>9.1666666666666661</v>
       </c>
-      <c r="E9">
-        <v>5.8387395736793328</v>
-      </c>
       <c r="F9">
+        <v>4.4366715758468338</v>
+      </c>
+      <c r="G9">
         <v>5.5459869100930073</v>
-      </c>
-      <c r="G9">
-        <v>4.4366715758468338</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -812,22 +828,22 @@
         <v>12</v>
       </c>
       <c r="B10">
+        <v>6.2539844447277826</v>
+      </c>
+      <c r="C10">
         <v>9.2418949561806691</v>
       </c>
-      <c r="C10">
-        <v>6.2539844447277826</v>
-      </c>
       <c r="D10">
+        <v>5.4167461377074195</v>
+      </c>
+      <c r="E10">
         <v>7.5826151652303304</v>
       </c>
-      <c r="E10">
-        <v>5.4167461377074195</v>
-      </c>
       <c r="F10">
+        <v>3.3505487411233057</v>
+      </c>
+      <c r="G10">
         <v>4.7131665403083147</v>
-      </c>
-      <c r="G10">
-        <v>3.3505487411233057</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -835,22 +851,22 @@
         <v>35</v>
       </c>
       <c r="B11">
+        <v>8.1961816984858462</v>
+      </c>
+      <c r="C11">
         <v>11.404353689077249</v>
       </c>
-      <c r="C11">
-        <v>8.1961816984858462</v>
-      </c>
       <c r="D11">
+        <v>6.8794827760379835</v>
+      </c>
+      <c r="E11">
         <v>11.33768352365416</v>
       </c>
-      <c r="E11">
-        <v>6.8794827760379835</v>
-      </c>
       <c r="F11">
+        <v>2.5814942296011338</v>
+      </c>
+      <c r="G11">
         <v>3.4856206771022933</v>
-      </c>
-      <c r="G11">
-        <v>2.5814942296011338</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -858,22 +874,22 @@
         <v>11</v>
       </c>
       <c r="B12">
+        <v>7.4586567667904156</v>
+      </c>
+      <c r="C12">
         <v>9.8066511987625677</v>
       </c>
-      <c r="C12">
-        <v>7.4586567667904156</v>
-      </c>
       <c r="D12">
+        <v>6.9936708860759493</v>
+      </c>
+      <c r="E12">
         <v>9.2930780559646546</v>
       </c>
-      <c r="E12">
-        <v>6.9936708860759493</v>
-      </c>
       <c r="F12">
+        <v>5.2606559974647444</v>
+      </c>
+      <c r="G12">
         <v>6.9197429382752942</v>
-      </c>
-      <c r="G12">
-        <v>5.2606559974647444</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -881,22 +897,22 @@
         <v>10</v>
       </c>
       <c r="B13">
+        <v>7.6281287246722282</v>
+      </c>
+      <c r="C13">
         <v>9.787143009947588</v>
       </c>
-      <c r="C13">
-        <v>7.6281287246722282</v>
-      </c>
       <c r="D13">
+        <v>7.4348407217643135</v>
+      </c>
+      <c r="E13">
         <v>9.5540732181312045</v>
       </c>
-      <c r="E13">
-        <v>7.4348407217643135</v>
-      </c>
       <c r="F13">
+        <v>4.8867095028745355</v>
+      </c>
+      <c r="G13">
         <v>6.4951045957947677</v>
-      </c>
-      <c r="G13">
-        <v>4.8867095028745355</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -904,22 +920,22 @@
         <v>13</v>
       </c>
       <c r="B14">
+        <v>12.451149686449151</v>
+      </c>
+      <c r="C14">
         <v>17.450263905805926</v>
       </c>
-      <c r="C14">
-        <v>12.451149686449151</v>
-      </c>
       <c r="D14">
+        <v>11.244083236581227</v>
+      </c>
+      <c r="E14">
         <v>16.580267558528426</v>
       </c>
-      <c r="E14">
-        <v>11.244083236581227</v>
-      </c>
       <c r="F14">
+        <v>6.8120624663435647</v>
+      </c>
+      <c r="G14">
         <v>9.9497066219614414</v>
-      </c>
-      <c r="G14">
-        <v>6.8120624663435647</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -927,22 +943,22 @@
         <v>14</v>
       </c>
       <c r="B15">
+        <v>8.4769399342564</v>
+      </c>
+      <c r="C15">
         <v>12.821855634110152</v>
       </c>
-      <c r="C15">
-        <v>8.4769399342564</v>
-      </c>
       <c r="D15">
+        <v>7.39047619047619</v>
+      </c>
+      <c r="E15">
         <v>12.350914391730718</v>
       </c>
-      <c r="E15">
-        <v>7.39047619047619</v>
-      </c>
       <c r="F15">
+        <v>4.8495471808355246</v>
+      </c>
+      <c r="G15">
         <v>6.586879432624114</v>
-      </c>
-      <c r="G15">
-        <v>4.8495471808355246</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -950,22 +966,22 @@
         <v>15</v>
       </c>
       <c r="B16">
+        <v>9.7028661582960822</v>
+      </c>
+      <c r="C16">
         <v>13.701107845353832</v>
       </c>
-      <c r="C16">
-        <v>9.7028661582960822</v>
-      </c>
       <c r="D16">
+        <v>10.095287149111511</v>
+      </c>
+      <c r="E16">
         <v>18.551631649530623</v>
       </c>
-      <c r="E16">
-        <v>10.095287149111511</v>
-      </c>
       <c r="F16">
+        <v>5.2202699261522785</v>
+      </c>
+      <c r="G16">
         <v>9.3159000700443606</v>
-      </c>
-      <c r="G16">
-        <v>5.2202699261522785</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -973,22 +989,22 @@
         <v>16</v>
       </c>
       <c r="B17">
+        <v>7.266465777012483</v>
+      </c>
+      <c r="C17">
         <v>7.4356358398847746</v>
       </c>
-      <c r="C17">
-        <v>7.266465777012483</v>
-      </c>
       <c r="D17">
+        <v>6.9249592169657426</v>
+      </c>
+      <c r="E17">
         <v>8.3060364997660265</v>
       </c>
-      <c r="E17">
-        <v>6.9249592169657426</v>
-      </c>
       <c r="F17">
+        <v>4.7038733214313435</v>
+      </c>
+      <c r="G17">
         <v>4.8870056497175147</v>
-      </c>
-      <c r="G17">
-        <v>4.7038733214313435</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -996,22 +1012,22 @@
         <v>17</v>
       </c>
       <c r="B18">
+        <v>21.016137165910237</v>
+      </c>
+      <c r="C18">
         <v>28.907313451305534</v>
       </c>
-      <c r="C18">
-        <v>21.016137165910237</v>
-      </c>
       <c r="D18">
+        <v>20.14686722728888</v>
+      </c>
+      <c r="E18">
         <v>28.078347067956528</v>
       </c>
-      <c r="E18">
-        <v>20.14686722728888</v>
-      </c>
       <c r="F18">
+        <v>12.455074978312059</v>
+      </c>
+      <c r="G18">
         <v>16.839506172839506</v>
-      </c>
-      <c r="G18">
-        <v>12.455074978312059</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1019,22 +1035,22 @@
         <v>18</v>
       </c>
       <c r="B19">
+        <v>12.511685883452788</v>
+      </c>
+      <c r="C19">
         <v>17.141551119914674</v>
       </c>
-      <c r="C19">
-        <v>12.511685883452788</v>
-      </c>
       <c r="D19">
+        <v>12.634612467768846</v>
+      </c>
+      <c r="E19">
         <v>18.989467256907343</v>
       </c>
-      <c r="E19">
-        <v>12.634612467768846</v>
-      </c>
       <c r="F19">
+        <v>9.8280485881053803</v>
+      </c>
+      <c r="G19">
         <v>13.404995257666771</v>
-      </c>
-      <c r="G19">
-        <v>9.8280485881053803</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1042,22 +1058,22 @@
         <v>19</v>
       </c>
       <c r="B20">
+        <v>11.77707676130389</v>
+      </c>
+      <c r="C20">
         <v>15.571465098440296</v>
       </c>
-      <c r="C20">
-        <v>11.77707676130389</v>
-      </c>
       <c r="D20">
+        <v>9.2048069547430327</v>
+      </c>
+      <c r="E20">
         <v>14.296296296296296</v>
       </c>
-      <c r="E20">
-        <v>9.2048069547430327</v>
-      </c>
       <c r="F20">
+        <v>5.9739596630074034</v>
+      </c>
+      <c r="G20">
         <v>8.4796788760662327</v>
-      </c>
-      <c r="G20">
-        <v>5.9739596630074034</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1065,22 +1081,22 @@
         <v>20</v>
       </c>
       <c r="B21">
+        <v>13.208308126638435</v>
+      </c>
+      <c r="C21">
         <v>18.341658341658341</v>
       </c>
-      <c r="C21">
-        <v>13.208308126638435</v>
-      </c>
       <c r="D21">
+        <v>12.153602533650039</v>
+      </c>
+      <c r="E21">
         <v>17.258480460226146</v>
       </c>
-      <c r="E21">
-        <v>12.153602533650039</v>
-      </c>
       <c r="F21">
+        <v>7.2516758074344905</v>
+      </c>
+      <c r="G21">
         <v>10.103576314246629</v>
-      </c>
-      <c r="G21">
-        <v>7.2516758074344905</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1088,22 +1104,22 @@
         <v>21</v>
       </c>
       <c r="B22">
+        <v>11.363636363636363</v>
+      </c>
+      <c r="C22">
         <v>14.437112577484504</v>
       </c>
-      <c r="C22">
-        <v>11.363636363636363</v>
-      </c>
       <c r="D22">
+        <v>12.127526568035007</v>
+      </c>
+      <c r="E22">
         <v>17.94921875</v>
       </c>
-      <c r="E22">
-        <v>12.127526568035007</v>
-      </c>
       <c r="F22">
+        <v>5.4630815194195481</v>
+      </c>
+      <c r="G22">
         <v>8.3735909822866343</v>
-      </c>
-      <c r="G22">
-        <v>5.4630815194195481</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1111,22 +1127,22 @@
         <v>22</v>
       </c>
       <c r="B23">
+        <v>8.5431979756597176</v>
+      </c>
+      <c r="C23">
         <v>11.774516344229486</v>
       </c>
-      <c r="C23">
-        <v>8.5431979756597176</v>
-      </c>
       <c r="D23">
+        <v>9.7373925168487094</v>
+      </c>
+      <c r="E23">
         <v>14.018388318009736</v>
       </c>
-      <c r="E23">
-        <v>9.7373925168487094</v>
-      </c>
       <c r="F23">
+        <v>4.712969525159461</v>
+      </c>
+      <c r="G23">
         <v>6.7372690401081572</v>
-      </c>
-      <c r="G23">
-        <v>4.712969525159461</v>
       </c>
     </row>
   </sheetData>
@@ -1136,54 +1152,89 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC6987C3-D7D0-4612-9312-3FC95439C468}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>5.0820358597586512</v>
+      </c>
+      <c r="C2">
         <v>2018</v>
       </c>
-      <c r="C1">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>6.9383371790964636</v>
+      </c>
+      <c r="C3">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>5.3081404621403312</v>
+      </c>
+      <c r="C4">
         <v>2019</v>
       </c>
-      <c r="D1">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>7.3993829011384404</v>
+      </c>
+      <c r="C5">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>4.499746112194682</v>
+      </c>
+      <c r="C6">
         <v>2020</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>6.9383371790964636</v>
-      </c>
-      <c r="C2">
-        <v>7.3993829011384404</v>
-      </c>
-      <c r="D2">
+      <c r="B7">
         <v>6.5510313355045664</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>5.0820358597586512</v>
-      </c>
-      <c r="C3">
-        <v>5.3081404621403312</v>
-      </c>
-      <c r="D3">
-        <v>4.499746112194682</v>
+      <c r="C7">
+        <v>2020</v>
       </c>
     </row>
   </sheetData>
@@ -1196,7 +1247,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,22 +1257,22 @@
         <v>23</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
       <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1229,22 +1280,22 @@
         <v>5</v>
       </c>
       <c r="B2">
+        <v>7.9432134370493737</v>
+      </c>
+      <c r="C2">
         <v>12.764542936288089</v>
       </c>
-      <c r="C2">
+      <c r="D2">
+        <v>8.6585536438662754</v>
+      </c>
+      <c r="E2">
+        <v>12.828617517548066</v>
+      </c>
+      <c r="F2">
         <v>7.9432134370493737</v>
       </c>
-      <c r="D2">
-        <v>12.828617517548066</v>
-      </c>
-      <c r="E2">
-        <v>8.6585536438662754</v>
-      </c>
-      <c r="F2">
+      <c r="G2">
         <v>12.186521234421885</v>
-      </c>
-      <c r="G2">
-        <v>7.9432134370493737</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1252,22 +1303,22 @@
         <v>6</v>
       </c>
       <c r="B3">
+        <v>8.9641434262948216</v>
+      </c>
+      <c r="C3">
         <v>9.6857290056671825</v>
       </c>
-      <c r="C3">
-        <v>8.9641434262948216</v>
-      </c>
       <c r="D3">
+        <v>7.5414781297134237</v>
+      </c>
+      <c r="E3">
         <v>10.484273589615576</v>
       </c>
-      <c r="E3">
-        <v>7.5414781297134237</v>
-      </c>
       <c r="F3">
+        <v>5.1045211473018961</v>
+      </c>
+      <c r="G3">
         <v>9.9798387096774182</v>
-      </c>
-      <c r="G3">
-        <v>5.1045211473018961</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1275,22 +1326,22 @@
         <v>32</v>
       </c>
       <c r="B4">
+        <v>6.739484080873809</v>
+      </c>
+      <c r="C4">
         <v>9.1669068895935428</v>
       </c>
-      <c r="C4">
-        <v>6.739484080873809</v>
-      </c>
       <c r="D4">
+        <v>5.689176688251619</v>
+      </c>
+      <c r="E4">
         <v>7.39505143174868</v>
       </c>
-      <c r="E4">
-        <v>5.689176688251619</v>
-      </c>
       <c r="F4">
+        <v>4.7663551401869162</v>
+      </c>
+      <c r="G4">
         <v>7.6154469349176344</v>
-      </c>
-      <c r="G4">
-        <v>4.7663551401869162</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1298,22 +1349,22 @@
         <v>7</v>
       </c>
       <c r="B5">
+        <v>7.0124178232286338</v>
+      </c>
+      <c r="C5">
         <v>9.157574673582543</v>
       </c>
-      <c r="C5">
-        <v>7.0124178232286338</v>
-      </c>
       <c r="D5">
+        <v>6.6631318487097912</v>
+      </c>
+      <c r="E5">
         <v>9.0398365679264554</v>
       </c>
-      <c r="E5">
-        <v>6.6631318487097912</v>
-      </c>
       <c r="F5">
+        <v>6.1685490877497831</v>
+      </c>
+      <c r="G5">
         <v>8.0741118476967539</v>
-      </c>
-      <c r="G5">
-        <v>6.1685490877497831</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1321,22 +1372,22 @@
         <v>8</v>
       </c>
       <c r="B6">
+        <v>7.5718758895530884</v>
+      </c>
+      <c r="C6">
         <v>12.607891491985205</v>
       </c>
-      <c r="C6">
-        <v>7.5718758895530884</v>
-      </c>
       <c r="D6">
+        <v>6.6619115549215397</v>
+      </c>
+      <c r="E6">
         <v>11.944110576923077</v>
       </c>
-      <c r="E6">
-        <v>6.6619115549215397</v>
-      </c>
       <c r="F6">
+        <v>3.1532805429864252</v>
+      </c>
+      <c r="G6">
         <v>6.8585425597060627</v>
-      </c>
-      <c r="G6">
-        <v>3.1532805429864252</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1344,22 +1395,22 @@
         <v>9</v>
       </c>
       <c r="B7">
+        <v>4.6239961061085424</v>
+      </c>
+      <c r="C7">
         <v>5.6209850107066384</v>
       </c>
-      <c r="C7">
-        <v>4.6239961061085424</v>
-      </c>
       <c r="D7">
+        <v>6.0493252675663101</v>
+      </c>
+      <c r="E7">
         <v>8.5151116951379766</v>
       </c>
-      <c r="E7">
-        <v>6.0493252675663101</v>
-      </c>
       <c r="F7">
+        <v>4.7205260685767971</v>
+      </c>
+      <c r="G7">
         <v>6.666666666666667</v>
-      </c>
-      <c r="G7">
-        <v>4.7205260685767971</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1367,22 +1418,22 @@
         <v>33</v>
       </c>
       <c r="B8">
+        <v>5.8321479374110954</v>
+      </c>
+      <c r="C8">
         <v>9.8670398880335899</v>
       </c>
-      <c r="C8">
-        <v>5.8321479374110954</v>
-      </c>
       <c r="D8">
+        <v>6.2229904926534134</v>
+      </c>
+      <c r="E8">
         <v>8.8872567021667273</v>
       </c>
-      <c r="E8">
-        <v>6.2229904926534134</v>
-      </c>
       <c r="F8">
+        <v>7.0339976553341153</v>
+      </c>
+      <c r="G8">
         <v>9.7560975609756095</v>
-      </c>
-      <c r="G8">
-        <v>7.0339976553341153</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1390,22 +1441,22 @@
         <v>34</v>
       </c>
       <c r="B9">
+        <v>6.303724928366762</v>
+      </c>
+      <c r="C9">
         <v>6.7457375833951074</v>
       </c>
-      <c r="C9">
-        <v>6.303724928366762</v>
-      </c>
       <c r="D9">
+        <v>5.7928613224107668</v>
+      </c>
+      <c r="E9">
         <v>6.5106071689831753</v>
       </c>
-      <c r="E9">
-        <v>5.7928613224107668</v>
-      </c>
       <c r="F9">
+        <v>4.6099290780141837</v>
+      </c>
+      <c r="G9">
         <v>7.5882794891059353</v>
-      </c>
-      <c r="G9">
-        <v>4.6099290780141837</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1413,22 +1464,22 @@
         <v>12</v>
       </c>
       <c r="B10">
+        <v>6.5536292627167079</v>
+      </c>
+      <c r="C10">
         <v>7.722792399146428</v>
       </c>
-      <c r="C10">
-        <v>6.5536292627167079</v>
-      </c>
       <c r="D10">
+        <v>4.9639165203822895</v>
+      </c>
+      <c r="E10">
         <v>7.5930067086806261</v>
       </c>
-      <c r="E10">
-        <v>4.9639165203822895</v>
-      </c>
       <c r="F10">
+        <v>3.5559495665878647</v>
+      </c>
+      <c r="G10">
         <v>5.355484470126922</v>
-      </c>
-      <c r="G10">
-        <v>3.5559495665878647</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1436,22 +1487,22 @@
         <v>35</v>
       </c>
       <c r="B11">
+        <v>6.1925689172992415</v>
+      </c>
+      <c r="C11">
         <v>8.3148148148148149</v>
       </c>
-      <c r="C11">
-        <v>6.1925689172992415</v>
-      </c>
       <c r="D11">
+        <v>6.9444444444444446</v>
+      </c>
+      <c r="E11">
         <v>9.1256935144442313</v>
       </c>
-      <c r="E11">
-        <v>6.9444444444444446</v>
-      </c>
       <c r="F11">
+        <v>3.9419934640522873</v>
+      </c>
+      <c r="G11">
         <v>5.3957548105534618</v>
-      </c>
-      <c r="G11">
-        <v>3.9419934640522873</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1459,22 +1510,22 @@
         <v>11</v>
       </c>
       <c r="B12">
+        <v>5.3733031674208149</v>
+      </c>
+      <c r="C12">
         <v>7.2605561277033992</v>
       </c>
-      <c r="C12">
-        <v>5.3733031674208149</v>
-      </c>
       <c r="D12">
+        <v>7.716049382716049</v>
+      </c>
+      <c r="E12">
         <v>10.107923137667807</v>
       </c>
-      <c r="E12">
-        <v>7.716049382716049</v>
-      </c>
       <c r="F12">
+        <v>6.7694944301628102</v>
+      </c>
+      <c r="G12">
         <v>8.8155759870200114</v>
-      </c>
-      <c r="G12">
-        <v>6.7694944301628102</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1482,22 +1533,22 @@
         <v>10</v>
       </c>
       <c r="B13">
+        <v>6.6824085005903182</v>
+      </c>
+      <c r="C13">
         <v>7.2465451167111841</v>
       </c>
-      <c r="C13">
-        <v>6.6824085005903182</v>
-      </c>
       <c r="D13">
+        <v>6.5503199534613143</v>
+      </c>
+      <c r="E13">
         <v>8.0588235294117645</v>
       </c>
-      <c r="E13">
-        <v>6.5503199534613143</v>
-      </c>
       <c r="F13">
+        <v>7.5762931542358896</v>
+      </c>
+      <c r="G13">
         <v>9.4788473329245857</v>
-      </c>
-      <c r="G13">
-        <v>7.5762931542358896</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1505,22 +1556,22 @@
         <v>13</v>
       </c>
       <c r="B14">
+        <v>9.7227497151538174</v>
+      </c>
+      <c r="C14">
         <v>13.03763440860215</v>
       </c>
-      <c r="C14">
-        <v>9.7227497151538174</v>
-      </c>
       <c r="D14">
+        <v>8.9509692132269105</v>
+      </c>
+      <c r="E14">
         <v>12.517059855722362</v>
       </c>
-      <c r="E14">
-        <v>8.9509692132269105</v>
-      </c>
       <c r="F14">
+        <v>7.5206301575393848</v>
+      </c>
+      <c r="G14">
         <v>11.172305271439811</v>
-      </c>
-      <c r="G14">
-        <v>7.5206301575393848</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1528,22 +1579,22 @@
         <v>14</v>
       </c>
       <c r="B15">
+        <v>6.5760631302060499</v>
+      </c>
+      <c r="C15">
         <v>9.4987411306935225</v>
       </c>
-      <c r="C15">
-        <v>6.5760631302060499</v>
-      </c>
       <c r="D15">
+        <v>7.2636600173460533</v>
+      </c>
+      <c r="E15">
         <v>11.372269705603038</v>
       </c>
-      <c r="E15">
-        <v>7.2636600173460533</v>
-      </c>
       <c r="F15">
+        <v>5.5724197745013013</v>
+      </c>
+      <c r="G15">
         <v>6.4218009478672986</v>
-      </c>
-      <c r="G15">
-        <v>5.5724197745013013</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1551,22 +1602,22 @@
         <v>15</v>
       </c>
       <c r="B16">
+        <v>6.5040650406504072</v>
+      </c>
+      <c r="C16">
         <v>10.060975609756099</v>
       </c>
-      <c r="C16">
-        <v>6.5040650406504072</v>
-      </c>
       <c r="D16">
+        <v>8.9989888776541953</v>
+      </c>
+      <c r="E16">
         <v>12.973533990659055</v>
       </c>
-      <c r="E16">
-        <v>8.9989888776541953</v>
-      </c>
       <c r="F16">
+        <v>6.0944641950228542</v>
+      </c>
+      <c r="G16">
         <v>10.974960042621204</v>
-      </c>
-      <c r="G16">
-        <v>6.0944641950228542</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1574,22 +1625,22 @@
         <v>16</v>
       </c>
       <c r="B17">
+        <v>4.1874376869391829</v>
+      </c>
+      <c r="C17">
         <v>5.7417706297910716</v>
       </c>
-      <c r="C17">
-        <v>4.1874376869391829</v>
-      </c>
       <c r="D17">
+        <v>4.7591633083861069</v>
+      </c>
+      <c r="E17">
         <v>7.398877213185548</v>
       </c>
-      <c r="E17">
-        <v>4.7591633083861069</v>
-      </c>
       <c r="F17">
+        <v>6.1040632469203899</v>
+      </c>
+      <c r="G17">
         <v>8.9112958168687832</v>
-      </c>
-      <c r="G17">
-        <v>6.1040632469203899</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1597,22 +1648,22 @@
         <v>17</v>
       </c>
       <c r="B18">
+        <v>12.709883103081829</v>
+      </c>
+      <c r="C18">
         <v>17.510959571358985</v>
       </c>
-      <c r="C18">
-        <v>12.709883103081829</v>
-      </c>
       <c r="D18">
+        <v>14.1961970613656</v>
+      </c>
+      <c r="E18">
         <v>22.483829236739975</v>
       </c>
-      <c r="E18">
-        <v>14.1961970613656</v>
-      </c>
       <c r="F18">
+        <v>11.373092926490985</v>
+      </c>
+      <c r="G18">
         <v>18.498583569405099</v>
-      </c>
-      <c r="G18">
-        <v>11.373092926490985</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1620,22 +1671,22 @@
         <v>18</v>
       </c>
       <c r="B19">
+        <v>9.5151672284158675</v>
+      </c>
+      <c r="C19">
         <v>13.271706833938593</v>
       </c>
-      <c r="C19">
-        <v>9.5151672284158675</v>
-      </c>
       <c r="D19">
+        <v>9.7757621567145367</v>
+      </c>
+      <c r="E19">
         <v>14.102564102564102</v>
       </c>
-      <c r="E19">
-        <v>9.7757621567145367</v>
-      </c>
       <c r="F19">
+        <v>8.8050314465408803</v>
+      </c>
+      <c r="G19">
         <v>12.726683937823836</v>
-      </c>
-      <c r="G19">
-        <v>8.8050314465408803</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1643,22 +1694,22 @@
         <v>19</v>
       </c>
       <c r="B20">
+        <v>6.5478496706702831</v>
+      </c>
+      <c r="C20">
         <v>10.498046875</v>
       </c>
-      <c r="C20">
-        <v>6.5478496706702831</v>
-      </c>
       <c r="D20">
+        <v>6.7619783616692422</v>
+      </c>
+      <c r="E20">
         <v>10.552027357107963</v>
       </c>
-      <c r="E20">
-        <v>6.7619783616692422</v>
-      </c>
       <c r="F20">
+        <v>8.557255064076065</v>
+      </c>
+      <c r="G20">
         <v>12.160804020100501</v>
-      </c>
-      <c r="G20">
-        <v>8.557255064076065</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1666,22 +1717,22 @@
         <v>20</v>
       </c>
       <c r="B21">
+        <v>8.9498018494055476</v>
+      </c>
+      <c r="C21">
         <v>13.678065054211844</v>
       </c>
-      <c r="C21">
-        <v>8.9498018494055476</v>
-      </c>
       <c r="D21">
+        <v>10.435630689206763</v>
+      </c>
+      <c r="E21">
         <v>14.721030042918454</v>
       </c>
-      <c r="E21">
-        <v>10.435630689206763</v>
-      </c>
       <c r="F21">
+        <v>11.283783783783784</v>
+      </c>
+      <c r="G21">
         <v>15.677782589865744</v>
-      </c>
-      <c r="G21">
-        <v>11.283783783783784</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1689,22 +1740,22 @@
         <v>21</v>
       </c>
       <c r="B22">
+        <v>10.754716981132075</v>
+      </c>
+      <c r="C22">
         <v>16.797556719022687</v>
       </c>
-      <c r="C22">
-        <v>10.754716981132075</v>
-      </c>
       <c r="D22">
+        <v>11.753661284265865</v>
+      </c>
+      <c r="E22">
         <v>16.808510638297872</v>
       </c>
-      <c r="E22">
-        <v>11.753661284265865</v>
-      </c>
       <c r="F22">
+        <v>7.3935772964899185</v>
+      </c>
+      <c r="G22">
         <v>10.418482999128161</v>
-      </c>
-      <c r="G22">
-        <v>7.3935772964899185</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1712,22 +1763,22 @@
         <v>22</v>
       </c>
       <c r="B23">
+        <v>5.5861526357199054</v>
+      </c>
+      <c r="C23">
         <v>6.7383216205043412</v>
       </c>
-      <c r="C23">
-        <v>5.5861526357199054</v>
-      </c>
       <c r="D23">
+        <v>7.6908099688473524</v>
+      </c>
+      <c r="E23">
         <v>10.44806937848441</v>
       </c>
-      <c r="E23">
-        <v>7.6908099688473524</v>
-      </c>
       <c r="F23">
+        <v>4.236252545824847</v>
+      </c>
+      <c r="G23">
         <v>6.6243194192377493</v>
-      </c>
-      <c r="G23">
-        <v>4.236252545824847</v>
       </c>
     </row>
   </sheetData>
@@ -1737,81 +1788,197 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59968286-92DD-4AAF-A29F-BCB417493B25}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>25</v>
       </c>
       <c r="B2">
         <v>43.848076597186918</v>
       </c>
       <c r="C2">
+        <v>2021</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>56.15192340281309</v>
       </c>
-      <c r="D2">
+      <c r="C3">
+        <v>2021</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
-      <c r="E2">
+      <c r="C4">
+        <v>2021</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
         <v>43.15789473684211</v>
       </c>
-      <c r="F2">
+      <c r="C5">
+        <v>2022</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
         <v>56.84210526315789</v>
       </c>
-      <c r="G2">
+      <c r="C6">
+        <v>2022</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C7">
+        <v>2022</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>45.526959852849522</v>
+      </c>
+      <c r="C8">
+        <v>2021</v>
+      </c>
+      <c r="D8" t="s">
         <v>24</v>
       </c>
-      <c r="B3">
-        <v>45.526959852849522</v>
-      </c>
-      <c r="C3">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9">
         <v>51.813791810447483</v>
       </c>
-      <c r="D3">
+      <c r="C9">
+        <v>2021</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
         <v>2.6592483367029982</v>
       </c>
-      <c r="E3">
+      <c r="C10">
+        <v>2021</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11">
         <v>45.606814280054586</v>
       </c>
-      <c r="F3">
+      <c r="C11">
+        <v>2022</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
         <v>52.046191545245115</v>
       </c>
-      <c r="G3">
+      <c r="C12">
+        <v>2022</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13">
         <v>2.3469941747002978</v>
+      </c>
+      <c r="C13">
+        <v>2022</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1821,97 +1988,250 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8B7C17-4320-4928-89D5-75AAD1FEFE7F}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>67.330111382494067</v>
+      </c>
+      <c r="C2">
+        <v>2021</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B3">
+        <v>32.669888617505933</v>
+      </c>
+      <c r="C3">
+        <v>2021</v>
+      </c>
+      <c r="D3" t="s">
         <v>27</v>
       </c>
-      <c r="B2">
-        <v>32.669888617505933</v>
-      </c>
-      <c r="C2">
-        <v>67.330111382494067</v>
-      </c>
-      <c r="D2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>68.638587738654905</v>
+      </c>
+      <c r="C4">
+        <v>2022</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
         <v>31.361412261345102</v>
       </c>
-      <c r="E2">
-        <v>68.638587738654905</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C5">
+        <v>2022</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>52.77468066025159</v>
+      </c>
+      <c r="C6">
+        <v>2021</v>
+      </c>
+      <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="B3">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
         <v>47.22531933974841</v>
       </c>
-      <c r="C3">
-        <v>52.77468066025159</v>
-      </c>
-      <c r="D3">
+      <c r="C7">
+        <v>2021</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>53.539171174652246</v>
+      </c>
+      <c r="C8">
+        <v>2022</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
         <v>46.460828825347761</v>
       </c>
-      <c r="E3">
-        <v>53.539171174652246</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C9">
+        <v>2022</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>50.161420500403551</v>
+      </c>
+      <c r="C10">
+        <v>2021</v>
+      </c>
+      <c r="D10" t="s">
         <v>29</v>
       </c>
-      <c r="B4">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11">
         <v>49.838579499596449</v>
       </c>
-      <c r="C4">
-        <v>50.161420500403551</v>
-      </c>
-      <c r="D4">
+      <c r="C11">
+        <v>2021</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>51.398135818908116</v>
+      </c>
+      <c r="C12">
+        <v>2022</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13">
         <v>48.601864181091877</v>
       </c>
-      <c r="E4">
-        <v>51.398135818908116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C13">
+        <v>2022</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>40.761478163493841</v>
+      </c>
+      <c r="C14">
+        <v>2021</v>
+      </c>
+      <c r="D14" t="s">
         <v>30</v>
       </c>
-      <c r="B5">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
         <v>59.238521836506166</v>
       </c>
-      <c r="C5">
-        <v>40.761478163493841</v>
-      </c>
-      <c r="D5">
+      <c r="C15">
+        <v>2021</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>43.494897959183675</v>
+      </c>
+      <c r="C16">
+        <v>2022</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17">
         <v>56.505102040816325</v>
       </c>
-      <c r="E5">
-        <v>43.494897959183675</v>
+      <c r="C17">
+        <v>2022</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1921,150 +2241,449 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F26A2421-B733-4CDF-9887-1A4DEF5AE21E}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>27</v>
       </c>
       <c r="B2">
         <v>33.250337609723161</v>
       </c>
       <c r="C2">
+        <v>2021</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>63.744935854152594</v>
       </c>
-      <c r="D2">
+      <c r="C3">
+        <v>2021</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
         <v>3.0047265361242403</v>
       </c>
-      <c r="E2">
+      <c r="C4">
+        <v>2021</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
         <v>30.941864629342248</v>
       </c>
-      <c r="F2">
+      <c r="C5">
+        <v>2022</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
         <v>67.267518204607853</v>
       </c>
-      <c r="G2">
+      <c r="C6">
+        <v>2022</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
         <v>1.7906171660498984</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C7">
+        <v>2022</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>47.100583951184305</v>
+      </c>
+      <c r="C8">
+        <v>2021</v>
+      </c>
+      <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="B3">
-        <v>47.100583951184305</v>
-      </c>
-      <c r="C3">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9">
         <v>50.001968374778563</v>
       </c>
-      <c r="D3">
+      <c r="C9">
+        <v>2021</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
         <v>2.8974476740371369</v>
       </c>
-      <c r="E3">
+      <c r="C10">
+        <v>2021</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11">
         <v>46.388886389606185</v>
       </c>
-      <c r="F3">
+      <c r="C11">
+        <v>2022</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
         <v>51.01085988321352</v>
       </c>
-      <c r="G3">
+      <c r="C12">
+        <v>2022</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13">
         <v>2.6002537271802995</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C13">
+        <v>2022</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>47.583361401145169</v>
+      </c>
+      <c r="C14">
+        <v>2021</v>
+      </c>
+      <c r="D14" t="s">
         <v>29</v>
       </c>
-      <c r="B4">
-        <v>47.583361401145169</v>
-      </c>
-      <c r="C4">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15">
         <v>51.473560121252945</v>
       </c>
-      <c r="D4">
+      <c r="C15">
+        <v>2021</v>
+      </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16">
         <v>0.94307847760188612</v>
       </c>
-      <c r="E4">
+      <c r="C16">
+        <v>2021</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17">
         <v>47.14045886961388</v>
       </c>
-      <c r="F4">
+      <c r="C17">
+        <v>2022</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18">
         <v>51.113598209289314</v>
       </c>
-      <c r="G4">
+      <c r="C18">
+        <v>2022</v>
+      </c>
+      <c r="D18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
         <v>1.7459429210968103</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C19">
+        <v>2022</v>
+      </c>
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>51.025641025641022</v>
+      </c>
+      <c r="C20">
+        <v>2021</v>
+      </c>
+      <c r="D20" t="s">
         <v>30</v>
       </c>
-      <c r="B5">
-        <v>51.025641025641022</v>
-      </c>
-      <c r="C5">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21">
         <v>46.92307692307692</v>
       </c>
-      <c r="D5">
+      <c r="C21">
+        <v>2021</v>
+      </c>
+      <c r="D21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22">
         <v>2.0512820512820511</v>
       </c>
-      <c r="E5">
+      <c r="C22">
+        <v>2021</v>
+      </c>
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23">
         <v>51.219512195121951</v>
       </c>
-      <c r="F5">
+      <c r="C23">
+        <v>2022</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24">
         <v>46.951219512195117</v>
       </c>
-      <c r="G5">
+      <c r="C24">
+        <v>2022</v>
+      </c>
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25">
         <v>1.8292682926829267</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C25">
+        <v>2022</v>
+      </c>
+      <c r="D25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>48.25665589840704</v>
+      </c>
+      <c r="C26">
+        <v>2021</v>
+      </c>
+      <c r="D26" t="s">
         <v>31</v>
       </c>
-      <c r="B6">
-        <v>48.25665589840704</v>
-      </c>
-      <c r="C6">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27">
         <v>51.74334410159296</v>
       </c>
-      <c r="D6">
+      <c r="C27">
+        <v>2021</v>
+      </c>
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28">
         <v>0</v>
       </c>
-      <c r="E6">
+      <c r="C28">
+        <v>2021</v>
+      </c>
+      <c r="D28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29">
         <v>48.379539242483403</v>
       </c>
-      <c r="F6">
+      <c r="C29">
+        <v>2022</v>
+      </c>
+      <c r="D29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30">
         <v>51.620460757516597</v>
       </c>
-      <c r="G6">
+      <c r="C30">
+        <v>2022</v>
+      </c>
+      <c r="D30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31">
         <v>0</v>
+      </c>
+      <c r="C31">
+        <v>2022</v>
+      </c>
+      <c r="D31" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2074,72 +2693,194 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF15D781-8068-4B3F-AFBC-034F56469321}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>61.428870731196319</v>
+      </c>
+      <c r="C2">
+        <v>2021</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="B3">
+        <v>38.571129268803688</v>
+      </c>
+      <c r="C3">
+        <v>2021</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>2021</v>
+      </c>
+      <c r="D4" t="s">
         <v>25</v>
       </c>
-      <c r="B2">
-        <v>38.571129268803688</v>
-      </c>
-      <c r="C2">
-        <v>61.428870731196319</v>
-      </c>
-      <c r="D2">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>50.642673521850902</v>
+      </c>
+      <c r="C5">
+        <v>2022</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
         <v>49.357326478149098</v>
       </c>
-      <c r="E2">
-        <v>50.642673521850902</v>
-      </c>
-      <c r="F2">
+      <c r="C6">
+        <v>2022</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C7">
+        <v>2022</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>60.660207410292614</v>
+      </c>
+      <c r="C8">
+        <v>2021</v>
+      </c>
+      <c r="D8" t="s">
         <v>24</v>
       </c>
-      <c r="B3">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
         <v>39.339792589707386</v>
       </c>
-      <c r="C3">
-        <v>60.660207410292614</v>
-      </c>
-      <c r="D3">
+      <c r="C9">
+        <v>2021</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10">
+        <v>2021</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>36.604774535809021</v>
+      </c>
+      <c r="C11">
+        <v>2022</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12">
         <v>24.250663129973475</v>
       </c>
-      <c r="E3">
-        <v>36.604774535809021</v>
-      </c>
-      <c r="F3">
+      <c r="C12">
+        <v>2022</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13">
         <v>39.144562334217511</v>
+      </c>
+      <c r="C13">
+        <v>2022</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -2149,97 +2890,250 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F6CB84-5A39-4B80-8609-30F46C4574D6}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>71.767515923566876</v>
+      </c>
+      <c r="C2">
+        <v>2021</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B3">
+        <v>28.232484076433124</v>
+      </c>
+      <c r="C3">
+        <v>2021</v>
+      </c>
+      <c r="D3" t="s">
         <v>27</v>
       </c>
-      <c r="B2">
-        <v>28.232484076433124</v>
-      </c>
-      <c r="C2">
-        <v>71.767515923566876</v>
-      </c>
-      <c r="D2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>72.932330827067673</v>
+      </c>
+      <c r="C4">
+        <v>2022</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
         <v>27.06766917293233</v>
       </c>
-      <c r="E2">
-        <v>72.932330827067673</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C5">
+        <v>2022</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>54.300595238095241</v>
+      </c>
+      <c r="C6">
+        <v>2021</v>
+      </c>
+      <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="B3">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
         <v>45.699404761904759</v>
       </c>
-      <c r="C3">
-        <v>54.300595238095241</v>
-      </c>
-      <c r="D3">
+      <c r="C7">
+        <v>2021</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>44.63519313304721</v>
+      </c>
+      <c r="C8">
+        <v>2022</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
         <v>55.36480686695279</v>
       </c>
-      <c r="E3">
-        <v>44.63519313304721</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C9">
+        <v>2022</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>48.489542989930285</v>
+      </c>
+      <c r="C10">
+        <v>2021</v>
+      </c>
+      <c r="D10" t="s">
         <v>29</v>
       </c>
-      <c r="B4">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11">
         <v>51.510457010069707</v>
       </c>
-      <c r="C4">
-        <v>48.489542989930285</v>
-      </c>
-      <c r="D4">
+      <c r="C11">
+        <v>2021</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>50.141643059490079</v>
+      </c>
+      <c r="C12">
+        <v>2022</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13">
         <v>49.858356940509914</v>
       </c>
-      <c r="E4">
-        <v>50.141643059490079</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C13">
+        <v>2022</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>2021</v>
+      </c>
+      <c r="D14" t="s">
         <v>30</v>
       </c>
-      <c r="B5">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
         <v>50</v>
       </c>
-      <c r="C5">
-        <v>50</v>
-      </c>
-      <c r="D5">
+      <c r="C15">
+        <v>2021</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>2022</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17">
         <v>80</v>
       </c>
-      <c r="E5">
-        <v>20</v>
+      <c r="C17">
+        <v>2022</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2249,132 +3143,446 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC803D0-7A11-4BE4-BA82-EB7906D3C273}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>67.330834484119151</v>
+      </c>
+      <c r="C2">
+        <v>2021</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="B3">
+        <v>32.669165515880842</v>
+      </c>
+      <c r="C3">
+        <v>2021</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>2021</v>
+      </c>
+      <c r="D4" t="s">
         <v>27</v>
       </c>
-      <c r="B2">
-        <v>32.669165515880842</v>
-      </c>
-      <c r="C2">
-        <v>67.330834484119151</v>
-      </c>
-      <c r="D2">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>60.512414157422079</v>
+      </c>
+      <c r="C5">
+        <v>2022</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
         <v>26.91494981510829</v>
       </c>
-      <c r="E2">
-        <v>60.512414157422079</v>
-      </c>
-      <c r="F2">
+      <c r="C6">
+        <v>2022</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
         <v>12.572636027469624</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C7">
+        <v>2022</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>59.305779512857505</v>
+      </c>
+      <c r="C8">
+        <v>2021</v>
+      </c>
+      <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="B3">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
         <v>40.694220487142495</v>
       </c>
-      <c r="C3">
-        <v>59.305779512857505</v>
-      </c>
-      <c r="D3">
+      <c r="C9">
+        <v>2021</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10">
+        <v>2021</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>29.935868071461293</v>
+      </c>
+      <c r="C11">
+        <v>2022</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12">
         <v>21.346770499312871</v>
       </c>
-      <c r="E3">
-        <v>29.935868071461293</v>
-      </c>
-      <c r="F3">
+      <c r="C12">
+        <v>2022</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13">
         <v>48.717361429225839</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C13">
+        <v>2022</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>53.618030842230134</v>
+      </c>
+      <c r="C14">
+        <v>2021</v>
+      </c>
+      <c r="D14" t="s">
         <v>29</v>
       </c>
-      <c r="B4">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
         <v>46.381969157769873</v>
       </c>
-      <c r="C4">
-        <v>53.618030842230134</v>
-      </c>
-      <c r="D4">
+      <c r="C15">
+        <v>2021</v>
+      </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16">
+        <v>2021</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>23.783287419651057</v>
+      </c>
+      <c r="C17">
+        <v>2022</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
         <v>23.048668503213957</v>
       </c>
-      <c r="E4">
-        <v>23.783287419651057</v>
-      </c>
-      <c r="F4">
+      <c r="C18">
+        <v>2022</v>
+      </c>
+      <c r="D18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
         <v>53.168044077134994</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C19">
+        <v>2022</v>
+      </c>
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>53.333333333333336</v>
+      </c>
+      <c r="C20">
+        <v>2021</v>
+      </c>
+      <c r="D20" t="s">
         <v>30</v>
       </c>
-      <c r="B5">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21">
         <v>46.666666666666664</v>
       </c>
-      <c r="C5">
-        <v>53.333333333333336</v>
-      </c>
-      <c r="D5">
+      <c r="C21">
+        <v>2021</v>
+      </c>
+      <c r="D21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22">
+        <v>2021</v>
+      </c>
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>4.5454545454545459</v>
+      </c>
+      <c r="C23">
+        <v>2022</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24">
         <v>27.27272727272727</v>
       </c>
-      <c r="E5">
-        <v>4.5454545454545459</v>
-      </c>
-      <c r="F5">
+      <c r="C24">
+        <v>2022</v>
+      </c>
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25">
         <v>68.181818181818173</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C25">
+        <v>2022</v>
+      </c>
+      <c r="D25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>82.10526315789474</v>
+      </c>
+      <c r="C26">
+        <v>2021</v>
+      </c>
+      <c r="D26" t="s">
         <v>31</v>
       </c>
-      <c r="B6">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27">
         <v>17.894736842105264</v>
       </c>
-      <c r="C6">
-        <v>82.10526315789474</v>
-      </c>
-      <c r="D6">
+      <c r="C27">
+        <v>2021</v>
+      </c>
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28">
+        <v>2021</v>
+      </c>
+      <c r="D28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>26.519337016574585</v>
+      </c>
+      <c r="C29">
+        <v>2022</v>
+      </c>
+      <c r="D29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30">
         <v>73.480662983425418</v>
       </c>
-      <c r="E6">
-        <v>26.519337016574585</v>
-      </c>
-      <c r="F6">
+      <c r="C30">
+        <v>2022</v>
+      </c>
+      <c r="D30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31">
         <v>0</v>
+      </c>
+      <c r="C31">
+        <v>2022</v>
+      </c>
+      <c r="D31" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -4575,29 +5783,26 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B99E45A1-6059-4E5D-B8B4-278C3E4BB526}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A3" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>2018</v>
-      </c>
-      <c r="C1">
-        <v>2019</v>
-      </c>
-      <c r="D1">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -4605,13 +5810,10 @@
         <v>5.1024340872759204</v>
       </c>
       <c r="C2">
-        <v>4.4797722683365269</v>
-      </c>
-      <c r="D2">
-        <v>1.4035035546061185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4619,10 +5821,51 @@
         <v>4.8401850257673429</v>
       </c>
       <c r="C3">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>4.4797722683365269</v>
+      </c>
+      <c r="C4">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
         <v>3.8653610519053943</v>
       </c>
-      <c r="D3">
+      <c r="C5">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1.4035035546061185</v>
+      </c>
+      <c r="C6">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
         <v>1.4204635335557376</v>
+      </c>
+      <c r="C7">
+        <v>2020</v>
       </c>
     </row>
   </sheetData>
@@ -4632,10 +5875,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F664417F-C21B-4C7F-8ABE-77D3ED054DD0}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4644,543 +5887,532 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1">
-        <v>2018</v>
-      </c>
-      <c r="D1">
-        <v>2019</v>
-      </c>
-      <c r="F1">
-        <v>2020</v>
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>3.1003512958175916</v>
+      </c>
+      <c r="C2">
+        <v>3.8139115790376996</v>
+      </c>
+      <c r="D2">
+        <v>2.5194305260625334</v>
+      </c>
+      <c r="E2">
+        <v>3.2541513499809862</v>
+      </c>
+      <c r="F2">
+        <v>0.8916268571091559</v>
+      </c>
+      <c r="G2">
+        <v>1.1444019627248956</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>3.8139115790376996</v>
+        <v>5.6512012450150761</v>
       </c>
       <c r="C3">
-        <v>3.1003512958175916</v>
+        <v>6.8612727614041678</v>
       </c>
       <c r="D3">
-        <v>3.2541513499809862</v>
+        <v>4.0103377595579719</v>
       </c>
       <c r="E3">
-        <v>2.5194305260625334</v>
+        <v>5.2453754540079398</v>
       </c>
       <c r="F3">
-        <v>1.1444019627248956</v>
+        <v>0.84792122538293224</v>
       </c>
       <c r="G3">
-        <v>0.8916268571091559</v>
+        <v>1.0874255631310952</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B4">
-        <v>6.8612727614041678</v>
+        <v>3.3750570110981606</v>
       </c>
       <c r="C4">
-        <v>5.6512012450150761</v>
+        <v>4.1135375445796081</v>
       </c>
       <c r="D4">
-        <v>5.2453754540079398</v>
+        <v>2.4307408665275823</v>
       </c>
       <c r="E4">
-        <v>4.0103377595579719</v>
+        <v>2.9798707637952675</v>
       </c>
       <c r="F4">
-        <v>1.0874255631310952</v>
+        <v>1.1479528994432675</v>
       </c>
       <c r="G4">
-        <v>0.84792122538293224</v>
+        <v>1.5527657164432698</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>4.1135375445796081</v>
+        <v>4.2014729870001482</v>
       </c>
       <c r="C5">
-        <v>3.3750570110981606</v>
+        <v>4.4916007786402634</v>
       </c>
       <c r="D5">
-        <v>2.9798707637952675</v>
+        <v>2.4846957148001438</v>
       </c>
       <c r="E5">
-        <v>2.4307408665275823</v>
+        <v>2.9954824510598863</v>
       </c>
       <c r="F5">
-        <v>1.5527657164432698</v>
+        <v>1.6042396048151168</v>
       </c>
       <c r="G5">
-        <v>1.1479528994432675</v>
+        <v>1.53138289219901</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>4.4916007786402634</v>
+        <v>7.8723251985972951</v>
       </c>
       <c r="C6">
-        <v>4.2014729870001482</v>
+        <v>9.1038471095850184</v>
       </c>
       <c r="D6">
-        <v>2.9954824510598863</v>
+        <v>5.8972881862211697</v>
       </c>
       <c r="E6">
-        <v>2.4846957148001438</v>
+        <v>7.0933939849318683</v>
       </c>
       <c r="F6">
-        <v>1.53138289219901</v>
+        <v>1.484225988205117</v>
       </c>
       <c r="G6">
-        <v>1.6042396048151168</v>
+        <v>1.5488624233417754</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>9.1038471095850184</v>
+        <v>4.278169014084507</v>
       </c>
       <c r="C7">
-        <v>7.8723251985972951</v>
+        <v>5.3985006491602796</v>
       </c>
       <c r="D7">
-        <v>7.0933939849318683</v>
+        <v>4.0609340549208257</v>
       </c>
       <c r="E7">
-        <v>5.8972881862211697</v>
+        <v>5.2078136393291636</v>
       </c>
       <c r="F7">
-        <v>1.5488624233417754</v>
+        <v>1.2668987290536713</v>
       </c>
       <c r="G7">
-        <v>1.484225988205117</v>
+        <v>1.5486552183799891</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B8">
-        <v>5.3985006491602796</v>
+        <v>2.7419049422457866</v>
       </c>
       <c r="C8">
-        <v>4.278169014084507</v>
+        <v>3.1938723896235275</v>
       </c>
       <c r="D8">
-        <v>5.2078136393291636</v>
+        <v>1.7885764243042401</v>
       </c>
       <c r="E8">
-        <v>4.0609340549208257</v>
+        <v>2.0606314613020396</v>
       </c>
       <c r="F8">
-        <v>1.5486552183799891</v>
+        <v>0.6317422787054825</v>
       </c>
       <c r="G8">
-        <v>1.2668987290536713</v>
+        <v>0.85932527052832597</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9">
-        <v>3.1938723896235275</v>
+        <v>5.025878993396395</v>
       </c>
       <c r="C9">
-        <v>2.7419049422457866</v>
+        <v>5.2249231628946635</v>
       </c>
       <c r="D9">
-        <v>2.0606314613020396</v>
+        <v>2.7806925498426023</v>
       </c>
       <c r="E9">
-        <v>1.7885764243042401</v>
+        <v>3.4430623324857397</v>
       </c>
       <c r="F9">
-        <v>0.85932527052832597</v>
+        <v>1.5367263499224588</v>
       </c>
       <c r="G9">
-        <v>0.6317422787054825</v>
+        <v>1.513157894736842</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="B10">
-        <v>5.2249231628946635</v>
+        <v>4.0197376338909612</v>
       </c>
       <c r="C10">
-        <v>5.025878993396395</v>
+        <v>4.5728410319789896</v>
       </c>
       <c r="D10">
-        <v>3.4430623324857397</v>
+        <v>2.8449502133712659</v>
       </c>
       <c r="E10">
-        <v>2.7806925498426023</v>
+        <v>3.4427687337797863</v>
       </c>
       <c r="F10">
-        <v>1.513157894736842</v>
+        <v>1.1593070209717338</v>
       </c>
       <c r="G10">
-        <v>1.5367263499224588</v>
+        <v>1.329367598251691</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B11">
-        <v>4.5728410319789896</v>
+        <v>7.307703673059307</v>
       </c>
       <c r="C11">
-        <v>4.0197376338909612</v>
+        <v>7.2707028531663189</v>
       </c>
       <c r="D11">
-        <v>3.4427687337797863</v>
+        <v>5.8054146922714551</v>
       </c>
       <c r="E11">
-        <v>2.8449502133712659</v>
+        <v>6.0700531817348242</v>
       </c>
       <c r="F11">
-        <v>1.329367598251691</v>
+        <v>1.8531458758420212</v>
       </c>
       <c r="G11">
-        <v>1.1593070209717338</v>
+        <v>1.6584669100142835</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>7.2707028531663189</v>
+        <v>5.956192509020684</v>
       </c>
       <c r="C12">
-        <v>7.307703673059307</v>
+        <v>6.4234002235071186</v>
       </c>
       <c r="D12">
-        <v>6.0700531817348242</v>
+        <v>4.089902464307591</v>
       </c>
       <c r="E12">
-        <v>5.8054146922714551</v>
+        <v>4.9402461237727131</v>
       </c>
       <c r="F12">
-        <v>1.6584669100142835</v>
+        <v>1.6446430269036982</v>
       </c>
       <c r="G12">
-        <v>1.8531458758420212</v>
+        <v>1.7360003645145123</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13">
-        <v>6.4234002235071186</v>
+        <v>4.8686774432582265</v>
       </c>
       <c r="C13">
-        <v>5.956192509020684</v>
+        <v>5.4691460128591629</v>
       </c>
       <c r="D13">
-        <v>4.9402461237727131</v>
+        <v>4.2177370672685752</v>
       </c>
       <c r="E13">
-        <v>4.089902464307591</v>
+        <v>5.1217154630783712</v>
       </c>
       <c r="F13">
-        <v>1.7360003645145123</v>
+        <v>1.2090401432936466</v>
       </c>
       <c r="G13">
-        <v>1.6446430269036982</v>
+        <v>1.3105070703454624</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>5.4691460128591629</v>
+        <v>8.798696665556772</v>
       </c>
       <c r="C14">
-        <v>4.8686774432582265</v>
+        <v>9.3519306395602886</v>
       </c>
       <c r="D14">
-        <v>5.1217154630783712</v>
+        <v>6.5365015745777271</v>
       </c>
       <c r="E14">
-        <v>4.2177370672685752</v>
+        <v>7.8050739674677017</v>
       </c>
       <c r="F14">
-        <v>1.3105070703454624</v>
+        <v>2.4304728188719067</v>
       </c>
       <c r="G14">
-        <v>1.2090401432936466</v>
+        <v>2.3062390305523572</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>9.3519306395602886</v>
+        <v>6.3840056161698895</v>
       </c>
       <c r="C15">
-        <v>8.798696665556772</v>
+        <v>6.3717435573344572</v>
       </c>
       <c r="D15">
-        <v>7.8050739674677017</v>
+        <v>4.6451960422986414</v>
       </c>
       <c r="E15">
-        <v>6.5365015745777271</v>
+        <v>5.4534313725490193</v>
       </c>
       <c r="F15">
-        <v>2.3062390305523572</v>
+        <v>2.0734242829882374</v>
       </c>
       <c r="G15">
-        <v>2.4304728188719067</v>
+        <v>1.8605096237970253</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>6.3717435573344572</v>
+        <v>5.2685671012062532</v>
       </c>
       <c r="C16">
-        <v>6.3840056161698895</v>
+        <v>5.5500956913050219</v>
       </c>
       <c r="D16">
-        <v>5.4534313725490193</v>
+        <v>5.2604672562752413</v>
       </c>
       <c r="E16">
-        <v>4.6451960422986414</v>
+        <v>5.9073377923155785</v>
       </c>
       <c r="F16">
-        <v>1.8605096237970253</v>
+        <v>1.8239325250395362</v>
       </c>
       <c r="G16">
-        <v>2.0734242829882374</v>
+        <v>1.6572088585346256</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>5.5500956913050219</v>
+        <v>6.1220357555473504</v>
       </c>
       <c r="C17">
-        <v>5.2685671012062532</v>
+        <v>4.9696041685711672</v>
       </c>
       <c r="D17">
-        <v>5.9073377923155785</v>
+        <v>4.0967016067935367</v>
       </c>
       <c r="E17">
-        <v>5.2604672562752413</v>
+        <v>4.0670605900208479</v>
       </c>
       <c r="F17">
-        <v>1.6572088585346256</v>
+        <v>2.3450793901215925</v>
       </c>
       <c r="G17">
-        <v>1.8239325250395362</v>
+        <v>1.7114387084946459</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>4.9696041685711672</v>
+        <v>12.049655172413793</v>
       </c>
       <c r="C18">
-        <v>6.1220357555473504</v>
+        <v>13.234290513937738</v>
       </c>
       <c r="D18">
-        <v>4.0670605900208479</v>
+        <v>11.052371541501977</v>
       </c>
       <c r="E18">
-        <v>4.0967016067935367</v>
+        <v>12.849333144823035</v>
       </c>
       <c r="F18">
-        <v>1.7114387084946459</v>
+        <v>3.2298294731483836</v>
       </c>
       <c r="G18">
-        <v>2.3450793901215925</v>
+        <v>3.4975728155339807</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>13.234290513937738</v>
+        <v>7.3390170117471412</v>
       </c>
       <c r="C19">
-        <v>12.049655172413793</v>
+        <v>8.4063834569566183</v>
       </c>
       <c r="D19">
-        <v>12.849333144823035</v>
+        <v>6.2803684096018566</v>
       </c>
       <c r="E19">
-        <v>11.052371541501977</v>
+        <v>7.6694739748722904</v>
       </c>
       <c r="F19">
-        <v>3.4975728155339807</v>
+        <v>1.7154426651941839</v>
       </c>
       <c r="G19">
-        <v>3.2298294731483836</v>
+        <v>1.7708773412195467</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>8.4063834569566183</v>
+        <v>8.0061264271790584</v>
       </c>
       <c r="C20">
-        <v>7.3390170117471412</v>
+        <v>9.7124893575217772</v>
       </c>
       <c r="D20">
-        <v>7.6694739748722904</v>
+        <v>5.2873712175208967</v>
       </c>
       <c r="E20">
-        <v>6.2803684096018566</v>
+        <v>6.6881106997633069</v>
       </c>
       <c r="F20">
-        <v>1.7708773412195467</v>
+        <v>2.1489320262286569</v>
       </c>
       <c r="G20">
-        <v>1.7154426651941839</v>
+        <v>2.4666995559940799</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>9.7124893575217772</v>
+        <v>6.1832959854153211</v>
       </c>
       <c r="C21">
-        <v>8.0061264271790584</v>
+        <v>7.1340757882557133</v>
       </c>
       <c r="D21">
-        <v>6.6881106997633069</v>
+        <v>6.1453515470940445</v>
       </c>
       <c r="E21">
-        <v>5.2873712175208967</v>
+        <v>7.958740124883569</v>
       </c>
       <c r="F21">
-        <v>2.4666995559940799</v>
+        <v>1.6722649618954744</v>
       </c>
       <c r="G21">
-        <v>2.1489320262286569</v>
+        <v>1.8525652250043774</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <v>7.1340757882557133</v>
+        <v>7.1412408924288364</v>
       </c>
       <c r="C22">
-        <v>6.1832959854153211</v>
+        <v>7.842203265058675</v>
       </c>
       <c r="D22">
-        <v>7.958740124883569</v>
+        <v>7.0850635729269236</v>
       </c>
       <c r="E22">
-        <v>6.1453515470940445</v>
+        <v>8.0318646573317451</v>
       </c>
       <c r="F22">
-        <v>1.8525652250043774</v>
+        <v>1.6673866090712741</v>
       </c>
       <c r="G22">
-        <v>1.6722649618954744</v>
+        <v>1.6203224068625419</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>7.842203265058675</v>
+        <v>4.4362610132158595</v>
       </c>
       <c r="C23">
-        <v>7.1412408924288364</v>
+        <v>5.2768622280817405</v>
       </c>
       <c r="D23">
-        <v>8.0318646573317451</v>
+        <v>4.6879021879021874</v>
       </c>
       <c r="E23">
-        <v>7.0850635729269236</v>
+        <v>6.1116576487948846</v>
       </c>
       <c r="F23">
-        <v>1.6203224068625419</v>
+        <v>1.3582453290008123</v>
       </c>
       <c r="G23">
-        <v>1.6673866090712741</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24">
-        <v>5.2768622280817405</v>
-      </c>
-      <c r="C24">
-        <v>4.4362610132158595</v>
-      </c>
-      <c r="D24">
-        <v>6.1116576487948846</v>
-      </c>
-      <c r="E24">
-        <v>4.6879021879021874</v>
-      </c>
-      <c r="F24">
         <v>1.5602747096243315</v>
-      </c>
-      <c r="G24">
-        <v>1.3582453290008123</v>
       </c>
     </row>
   </sheetData>
@@ -5190,54 +6422,89 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FEE7359-0537-4A70-933A-E49107758F45}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>6.0673365351517035</v>
+      </c>
+      <c r="C2">
         <v>2018</v>
       </c>
-      <c r="C1">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>7.9125983505545543</v>
+      </c>
+      <c r="C3">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>5.7490037589432985</v>
+      </c>
+      <c r="C4">
         <v>2019</v>
       </c>
-      <c r="D1">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>7.9634743494847111</v>
+      </c>
+      <c r="C5">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>3.8370582553375749</v>
+      </c>
+      <c r="C6">
         <v>2020</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>7.9125983505545543</v>
-      </c>
-      <c r="C2">
-        <v>7.9634743494847111</v>
-      </c>
-      <c r="D2">
+      <c r="B7">
         <v>5.1787197639386537</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>6.0673365351517035</v>
-      </c>
-      <c r="C3">
-        <v>5.7490037589432985</v>
-      </c>
-      <c r="D3">
-        <v>3.8370582553375749</v>
+      <c r="C7">
+        <v>2020</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version final POA 31-05-2023 15:15
</commit_message>
<xml_diff>
--- a/Codigo/Bases/datos_administrativos/Indicadores_de_Género/EDUCACIÓN/EducaciónSinFormato.xlsx
+++ b/Codigo/Bases/datos_administrativos/Indicadores_de_Género/EDUCACIÓN/EducaciónSinFormato.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pgalvez\OneDrive - ine.gob.gt\Documentos\GitHub\CompendioGenero2023\Codigo\Bases\datos_administrativos\Indicadores_de_Género\EDUCACIÓN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B28BF3E-5FDC-45AA-B485-A4F6AAA482F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64E7434-D8A3-4E2B-972C-7B8EDB945996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="8" activeTab="18" xr2:uid="{47FD8A6C-84B7-4DDA-B99C-2C5D2BD14377}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{47FD8A6C-84B7-4DDA-B99C-2C5D2BD14377}"/>
   </bookViews>
   <sheets>
     <sheet name="3.4" sheetId="20" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="42">
   <si>
     <t>Sexo</t>
   </si>
@@ -542,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71CC9C9D-F8C0-46A6-BEE4-E06341FE6022}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,6 +603,17 @@
       </c>
       <c r="C5" s="1">
         <v>92.284136104897001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2022</v>
+      </c>
+      <c r="B6" s="1">
+        <v>92.684981144130163</v>
+      </c>
+      <c r="C6" s="1">
+        <v>91.778116721522039</v>
       </c>
     </row>
   </sheetData>
@@ -2936,7 +2947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC803D0-7A11-4BE4-BA82-EB7906D3C273}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -3087,10 +3098,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64CF2CFD-E47A-4150-9670-BFC206BC7550}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3100,7 +3111,7 @@
     <col min="3" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -3128,8 +3139,14 @@
       <c r="I1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3157,8 +3174,15 @@
       <c r="I2" s="2">
         <v>99.482101158979404</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="2">
+        <v>98.82192721193131</v>
+      </c>
+      <c r="K2" s="2">
+        <v>97.882958856297648</v>
+      </c>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3186,8 +3210,15 @@
       <c r="I3" s="2">
         <v>103.52174678640607</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="2">
+        <v>96.885995777621389</v>
+      </c>
+      <c r="K3" s="2">
+        <v>101.39400315623357</v>
+      </c>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -3215,8 +3246,15 @@
       <c r="I4" s="2">
         <v>96.547863407352125</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="2">
+        <v>96.185405880629091</v>
+      </c>
+      <c r="K4" s="2">
+        <v>95.835670218732474</v>
+      </c>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -3244,8 +3282,15 @@
       <c r="I5" s="2">
         <v>92.836084905660371</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="2">
+        <v>91.773699632085652</v>
+      </c>
+      <c r="K5" s="2">
+        <v>89.803517334230904</v>
+      </c>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -3273,8 +3318,15 @@
       <c r="I6" s="2">
         <v>100.6711266405318</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="2">
+        <v>96.202340668577719</v>
+      </c>
+      <c r="K6" s="2">
+        <v>97.641320184977928</v>
+      </c>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -3302,8 +3354,15 @@
       <c r="I7" s="2">
         <v>94.366197183098592</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="2">
+        <v>92.998724933348782</v>
+      </c>
+      <c r="K7" s="2">
+        <v>92.138608740625799</v>
+      </c>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -3331,8 +3390,15 @@
       <c r="I8" s="2">
         <v>94.491511121612049</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="2">
+        <v>95.298901412469689</v>
+      </c>
+      <c r="K8" s="2">
+        <v>93.875123211311646</v>
+      </c>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -3360,8 +3426,15 @@
       <c r="I9" s="2">
         <v>83.338170420246115</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="2">
+        <v>87.394270122783084</v>
+      </c>
+      <c r="K9" s="2">
+        <v>84.819827636069178</v>
+      </c>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3389,8 +3462,15 @@
       <c r="I10" s="2">
         <v>94.036216058193318</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="2">
+        <v>92.097290746992115</v>
+      </c>
+      <c r="K10" s="2">
+        <v>92.37833341820712</v>
+      </c>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -3418,8 +3498,15 @@
       <c r="I11" s="2">
         <v>92.39135712551591</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="2">
+        <v>93.128699734639724</v>
+      </c>
+      <c r="K11" s="2">
+        <v>92.525014714537974</v>
+      </c>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -3447,8 +3534,15 @@
       <c r="I12" s="2">
         <v>91.273164462501555</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="2">
+        <v>91.18911803422553</v>
+      </c>
+      <c r="K12" s="2">
+        <v>89.065451260573212</v>
+      </c>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -3476,8 +3570,15 @@
       <c r="I13" s="2">
         <v>90.681760189287616</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="2">
+        <v>91.339878957279737</v>
+      </c>
+      <c r="K13" s="2">
+        <v>91.001941613722266</v>
+      </c>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -3505,8 +3606,15 @@
       <c r="I14" s="2">
         <v>83.069812247015136</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="2">
+        <v>87.502268754238983</v>
+      </c>
+      <c r="K14" s="2">
+        <v>84.508107123337581</v>
+      </c>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -3534,8 +3642,15 @@
       <c r="I15" s="2">
         <v>88.077596335995011</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="2">
+        <v>89.563899688233619</v>
+      </c>
+      <c r="K15" s="2">
+        <v>89.027294812556562</v>
+      </c>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -3563,8 +3678,15 @@
       <c r="I16" s="2">
         <v>86.174896408839771</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="2">
+        <v>85.102404274265368</v>
+      </c>
+      <c r="K16" s="2">
+        <v>86.491235589079835</v>
+      </c>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -3592,8 +3714,15 @@
       <c r="I17" s="2">
         <v>90.565411390242232</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="2">
+        <v>91.781846497474405</v>
+      </c>
+      <c r="K17" s="2">
+        <v>91.038726519716576</v>
+      </c>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -3621,8 +3750,15 @@
       <c r="I18" s="2">
         <v>91.590130226182325</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="2">
+        <v>92.694513087497896</v>
+      </c>
+      <c r="K18" s="2">
+        <v>91.34937902275405</v>
+      </c>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -3650,8 +3786,15 @@
       <c r="I19" s="2">
         <v>95.984977808125635</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="2">
+        <v>95.129031116145697</v>
+      </c>
+      <c r="K19" s="2">
+        <v>94.304653679653683</v>
+      </c>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -3679,8 +3822,15 @@
       <c r="I20" s="2">
         <v>93.254104948903432</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="2">
+        <v>90.590373453714008</v>
+      </c>
+      <c r="K20" s="2">
+        <v>91.894970666970437</v>
+      </c>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -3708,8 +3858,15 @@
       <c r="I21" s="2">
         <v>90.760852256441297</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="2">
+        <v>91.603832603470408</v>
+      </c>
+      <c r="K21" s="2">
+        <v>91.702391159378877</v>
+      </c>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -3737,8 +3894,15 @@
       <c r="I22" s="2">
         <v>88.659074210139593</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="2">
+        <v>90.194879633167744</v>
+      </c>
+      <c r="K22" s="2">
+        <v>89.048335596579449</v>
+      </c>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -3766,6 +3930,24 @@
       <c r="I23" s="2">
         <v>91.558176192422209</v>
       </c>
+      <c r="J23" s="2">
+        <v>93.421133044062827</v>
+      </c>
+      <c r="K23" s="2">
+        <v>90.496973929236503</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3774,10 +3956,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D10DC42-1B06-4E18-98AB-81776622FEF6}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3834,6 +4016,17 @@
         <v>43.855576665754903</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2022</v>
+      </c>
+      <c r="B6">
+        <v>47.728568858677143</v>
+      </c>
+      <c r="C6">
+        <v>46.214180651138413</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3841,10 +4034,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF93E2F7-8EF3-4D4D-A775-68B654942920}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A23"/>
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3852,7 +4045,7 @@
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -3880,8 +4073,14 @@
       <c r="I1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3909,8 +4108,14 @@
       <c r="I2">
         <v>74.158610239665364</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>82.437718070093553</v>
+      </c>
+      <c r="K2">
+        <v>78.015028244953967</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3938,8 +4143,14 @@
       <c r="I3">
         <v>55.756671020712822</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>61.382799325463743</v>
+      </c>
+      <c r="K3">
+        <v>60.357675111773467</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -3967,8 +4178,14 @@
       <c r="I4">
         <v>59.389038634321658</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>65.721481205111459</v>
+      </c>
+      <c r="K4">
+        <v>61.912494361750113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -3996,8 +4213,14 @@
       <c r="I5">
         <v>43.223581851057567</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>46.333244657267002</v>
+      </c>
+      <c r="K5">
+        <v>43.394168239983216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -4025,8 +4248,14 @@
       <c r="I6">
         <v>53.878661087866107</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>56.800242865816642</v>
+      </c>
+      <c r="K6">
+        <v>56.761573386515039</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -4054,8 +4283,14 @@
       <c r="I7">
         <v>51.80325352977286</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>59.082878252489557</v>
+      </c>
+      <c r="K7">
+        <v>53.361473522640054</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -4083,8 +4318,14 @@
       <c r="I8">
         <v>41.007512152010605</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>45.409379968203496</v>
+      </c>
+      <c r="K8">
+        <v>42.20936148562707</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -4112,8 +4353,14 @@
       <c r="I9">
         <v>28.008223485306566</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>31.503655155028987</v>
+      </c>
+      <c r="K9">
+        <v>29.5803603821502</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -4141,8 +4388,14 @@
       <c r="I10">
         <v>52.218973239071701</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>55.961510101754911</v>
+      </c>
+      <c r="K10">
+        <v>55.333108386758148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -4170,8 +4423,14 @@
       <c r="I11">
         <v>42.016951340188449</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>42.598714416896236</v>
+      </c>
+      <c r="K11">
+        <v>43.263984385396796</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -4199,8 +4458,14 @@
       <c r="I12">
         <v>50.70317050844637</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>55.153707052441227</v>
+      </c>
+      <c r="K12">
+        <v>52.127127127127125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -4228,8 +4493,14 @@
       <c r="I13">
         <v>37.999904666571332</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>43.848768265151705</v>
+      </c>
+      <c r="K13">
+        <v>41.80558247722427</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -4257,8 +4528,14 @@
       <c r="I14">
         <v>20.733016725170351</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>23.872160479398204</v>
+      </c>
+      <c r="K14">
+        <v>22.747697375109286</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -4286,8 +4563,14 @@
       <c r="I15">
         <v>25.042779362198598</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>26.245802909982412</v>
+      </c>
+      <c r="K15">
+        <v>25.82018404751587</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -4315,8 +4598,14 @@
       <c r="I16">
         <v>33.448057241191918</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>36.380597014925378</v>
+      </c>
+      <c r="K16">
+        <v>36.262744744202834</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -4344,8 +4633,14 @@
       <c r="I17">
         <v>33.94590699054644</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>27.95968169761273</v>
+      </c>
+      <c r="K17">
+        <v>35.285379997965208</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -4373,8 +4668,14 @@
       <c r="I18">
         <v>30.140748369378645</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>40.407111569183201</v>
+      </c>
+      <c r="K18">
+        <v>35.103130308177626</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -4402,8 +4703,14 @@
       <c r="I19">
         <v>38.399495020339458</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <v>44.918250110472826</v>
+      </c>
+      <c r="K19">
+        <v>43.339720388900716</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -4431,8 +4738,14 @@
       <c r="I20">
         <v>45.202143205065759</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <v>50.0062134957127</v>
+      </c>
+      <c r="K20">
+        <v>46.747572815533985</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -4460,8 +4773,14 @@
       <c r="I21">
         <v>29.235372340425531</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <v>33.335595520868679</v>
+      </c>
+      <c r="K21">
+        <v>30.158204805719201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -4489,8 +4808,14 @@
       <c r="I22">
         <v>31.413377275110477</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <v>36.277529647312491</v>
+      </c>
+      <c r="K22">
+        <v>34.164310165203155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -4517,6 +4842,12 @@
       </c>
       <c r="I23">
         <v>46.377745241581259</v>
+      </c>
+      <c r="J23">
+        <v>50.943750000000001</v>
+      </c>
+      <c r="K23">
+        <v>49.328020932445291</v>
       </c>
     </row>
   </sheetData>
@@ -4526,10 +4857,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06C7E90-ABCF-4680-81A1-E35771116289}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4586,6 +4917,17 @@
         <v>21.570622148844869</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2022</v>
+      </c>
+      <c r="B6">
+        <v>25.574285338104204</v>
+      </c>
+      <c r="C6">
+        <v>21.676596335942648</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4593,10 +4935,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F975AF-F4EC-4D19-AB1E-42A7AC4A093B}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4604,7 +4946,7 @@
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -4632,8 +4974,14 @@
       <c r="I1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4661,8 +5009,14 @@
       <c r="I2">
         <v>43.915796309324094</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>53.051128818061088</v>
+      </c>
+      <c r="K2">
+        <v>46.315982999340306</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4690,8 +5044,14 @@
       <c r="I3">
         <v>31.092278719397363</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>34.478021978021978</v>
+      </c>
+      <c r="K3">
+        <v>31.082118188795089</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -4719,8 +5079,14 @@
       <c r="I4">
         <v>29.263977353149329</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>36.982274873073841</v>
+      </c>
+      <c r="K4">
+        <v>30.749491195469425</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -4748,8 +5114,14 @@
       <c r="I5">
         <v>21.300411522633745</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>23.77201522258607</v>
+      </c>
+      <c r="K5">
+        <v>20.869312520757223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -4777,8 +5149,14 @@
       <c r="I6">
         <v>24.534923050904787</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>29.971879731775903</v>
+      </c>
+      <c r="K6">
+        <v>25.149700598802394</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -4806,8 +5184,14 @@
       <c r="I7">
         <v>23.462154127601188</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>32.192982456140349</v>
+      </c>
+      <c r="K7">
+        <v>24.032789397073469</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -4835,8 +5219,14 @@
       <c r="I8">
         <v>13.688434405540095</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>19.846621710961259</v>
+      </c>
+      <c r="K8">
+        <v>13.860686287109624</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -4864,8 +5254,14 @@
       <c r="I9">
         <v>6.9777721646880524</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>9.7240134124322939</v>
+      </c>
+      <c r="K9">
+        <v>7.4555618365680543</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -4893,8 +5289,14 @@
       <c r="I10">
         <v>26.755025253381241</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>27.82474260715108</v>
+      </c>
+      <c r="K10">
+        <v>25.316895294321927</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -4922,8 +5324,14 @@
       <c r="I11">
         <v>19.260139924093465</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>22.203618436351796</v>
+      </c>
+      <c r="K11">
+        <v>18.816868758915835</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -4951,8 +5359,14 @@
       <c r="I12">
         <v>27.419354838709676</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>32.176858293665319</v>
+      </c>
+      <c r="K12">
+        <v>27.123195703256126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -4980,8 +5394,14 @@
       <c r="I13">
         <v>16.228399699474082</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>18.012452573207511</v>
+      </c>
+      <c r="K13">
+        <v>15.649174909587336</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -5009,8 +5429,14 @@
       <c r="I14">
         <v>8.9520651059280443</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>11.572307277870067</v>
+      </c>
+      <c r="K14">
+        <v>8.3275876928380601</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -5038,8 +5464,14 @@
       <c r="I15">
         <v>9.3562813389348154</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>11.892321671967288</v>
+      </c>
+      <c r="K15">
+        <v>8.5240320968308421</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -5067,8 +5499,14 @@
       <c r="I16">
         <v>13.672795851013673</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>17.653328165875401</v>
+      </c>
+      <c r="K16">
+        <v>13.787623854926153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -5096,8 +5534,14 @@
       <c r="I17">
         <v>13.889766623030741</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>11.799079073463759</v>
+      </c>
+      <c r="K17">
+        <v>13.145624103299857</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -5125,8 +5569,14 @@
       <c r="I18">
         <v>13.718787158145066</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>19.783633247643532</v>
+      </c>
+      <c r="K18">
+        <v>13.356061365687401</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -5154,8 +5604,14 @@
       <c r="I19">
         <v>17.571993994813702</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <v>24.465336586766185</v>
+      </c>
+      <c r="K19">
+        <v>17.64256442314371</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -5183,8 +5639,14 @@
       <c r="I20">
         <v>23.019468593118646</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <v>28.59831848412599</v>
+      </c>
+      <c r="K20">
+        <v>23.59633935196636</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -5212,8 +5674,14 @@
       <c r="I21">
         <v>12.568639414276998</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <v>18.185586955019691</v>
+      </c>
+      <c r="K21">
+        <v>12.115646258503402</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -5241,8 +5709,14 @@
       <c r="I22">
         <v>13.14987040707425</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <v>18.370089321002293</v>
+      </c>
+      <c r="K22">
+        <v>13.124425375421392</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -5269,6 +5743,12 @@
       </c>
       <c r="I23">
         <v>22.281014551101396</v>
+      </c>
+      <c r="J23">
+        <v>28.00927338173388</v>
+      </c>
+      <c r="K23">
+        <v>21.79220178178873</v>
       </c>
     </row>
   </sheetData>

</xml_diff>